<commit_message>
fix: :card_file_box: FIX DATA 2018
</commit_message>
<xml_diff>
--- a/apps/load_data/2018/01/PLMOVMAE.xlsx
+++ b/apps/load_data/2018/01/PLMOVMAE.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOMBRADOS -2018\HHY0118\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACTUALIZADOS\2018\HHY0118\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C45D28-29C6-4F31-962A-BA85D0944B0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8843BEE3-281E-4A87-9F96-422D9E299FCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLMOVMAE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLMOVMAE!$A$1:$CF$264</definedName>
     <definedName name="_xlnm.Database">PLMOVMAE!$A$1:$CF$264</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10534" uniqueCount="2639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10521" uniqueCount="2637">
   <si>
     <t>CODEJE</t>
   </si>
@@ -6511,9 +6512,6 @@
     <t>08771747</t>
   </si>
   <si>
-    <t>S/N</t>
-  </si>
-  <si>
     <t>1047    134900    1349001056     40000     400001081    326625    3266251082    175875    1758752001         0     424612006     46100     461002026    353303    3533032027      3068      30682029      1500      15002086      2500      2500</t>
   </si>
   <si>
@@ -7847,9 +7845,6 @@
   </si>
   <si>
     <t>06567208</t>
-  </si>
-  <si>
-    <t>S/M</t>
   </si>
   <si>
     <t>6501080BIHTE003</t>
@@ -7945,7 +7940,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -8785,10 +8780,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC271" sqref="AC271"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45170,12 +45167,7 @@
       <c r="AA209" s="1">
         <v>0</v>
       </c>
-      <c r="AC209" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD209" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC209" s="3"/>
       <c r="AF209" s="1" t="s">
         <v>103</v>
       </c>
@@ -45240,10 +45232,10 @@
         <v>110</v>
       </c>
       <c r="BH209" s="1" t="s">
+        <v>2162</v>
+      </c>
+      <c r="BI209" s="1" t="s">
         <v>2163</v>
-      </c>
-      <c r="BI209" s="1" t="s">
-        <v>2164</v>
       </c>
       <c r="BM209" s="1" t="s">
         <v>113</v>
@@ -45255,7 +45247,7 @@
         <v>152</v>
       </c>
       <c r="BT209" s="1" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="BU209" s="1" t="s">
         <v>117</v>
@@ -45276,13 +45268,13 @@
         <v>98</v>
       </c>
       <c r="CC209" s="1" t="s">
+        <v>2165</v>
+      </c>
+      <c r="CD209" s="1" t="s">
         <v>2166</v>
       </c>
-      <c r="CD209" s="1" t="s">
+      <c r="CE209" s="1" t="s">
         <v>2167</v>
-      </c>
-      <c r="CE209" s="1" t="s">
-        <v>2168</v>
       </c>
     </row>
     <row r="210" spans="1:83" x14ac:dyDescent="0.25">
@@ -45317,13 +45309,13 @@
         <v>93</v>
       </c>
       <c r="K210" s="1" t="s">
+        <v>2168</v>
+      </c>
+      <c r="L210" s="1" t="s">
         <v>2169</v>
       </c>
-      <c r="L210" s="1" t="s">
+      <c r="N210" s="1" t="s">
         <v>2170</v>
-      </c>
-      <c r="N210" s="1" t="s">
-        <v>2171</v>
       </c>
       <c r="O210" s="1" t="s">
         <v>97</v>
@@ -45355,12 +45347,7 @@
       <c r="AB210" s="1" t="s">
         <v>1130</v>
       </c>
-      <c r="AC210" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD210" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC210" s="3"/>
       <c r="AF210" s="1" t="s">
         <v>103</v>
       </c>
@@ -45407,7 +45394,7 @@
         <v>98</v>
       </c>
       <c r="AZ210" s="1" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="BB210" s="1">
         <v>1</v>
@@ -45425,10 +45412,10 @@
         <v>110</v>
       </c>
       <c r="BH210" s="1" t="s">
+        <v>2172</v>
+      </c>
+      <c r="BI210" s="1" t="s">
         <v>2173</v>
-      </c>
-      <c r="BI210" s="1" t="s">
-        <v>2174</v>
       </c>
       <c r="BM210" s="1" t="s">
         <v>113</v>
@@ -45440,13 +45427,13 @@
         <v>99</v>
       </c>
       <c r="BR210" s="1" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="BS210" s="3">
         <v>36949</v>
       </c>
       <c r="BT210" s="1" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="BU210" s="1" t="s">
         <v>117</v>
@@ -45470,13 +45457,13 @@
         <v>98</v>
       </c>
       <c r="CC210" s="1" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="CD210" s="1" t="s">
         <v>1800</v>
       </c>
       <c r="CE210" s="1" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="211" spans="1:83" x14ac:dyDescent="0.25">
@@ -45511,13 +45498,13 @@
         <v>93</v>
       </c>
       <c r="K211" s="1" t="s">
+        <v>2178</v>
+      </c>
+      <c r="L211" s="1" t="s">
         <v>2179</v>
       </c>
-      <c r="L211" s="1" t="s">
+      <c r="N211" s="1" t="s">
         <v>2180</v>
-      </c>
-      <c r="N211" s="1" t="s">
-        <v>2181</v>
       </c>
       <c r="O211" s="1" t="s">
         <v>97</v>
@@ -45549,12 +45536,7 @@
       <c r="AB211" s="1" t="s">
         <v>1130</v>
       </c>
-      <c r="AC211" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD211" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC211" s="3"/>
       <c r="AF211" s="1" t="s">
         <v>103</v>
       </c>
@@ -45601,7 +45583,7 @@
         <v>98</v>
       </c>
       <c r="AZ211" s="1" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="BB211" s="1">
         <v>1</v>
@@ -45622,10 +45604,10 @@
         <v>110</v>
       </c>
       <c r="BH211" s="1" t="s">
+        <v>2182</v>
+      </c>
+      <c r="BI211" s="1" t="s">
         <v>2183</v>
-      </c>
-      <c r="BI211" s="1" t="s">
-        <v>2184</v>
       </c>
       <c r="BM211" s="1" t="s">
         <v>113</v>
@@ -45637,13 +45619,13 @@
         <v>99</v>
       </c>
       <c r="BR211" s="1" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="BS211" s="3">
         <v>36825</v>
       </c>
       <c r="BT211" s="1" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="BU211" s="1" t="s">
         <v>117</v>
@@ -45667,13 +45649,13 @@
         <v>98</v>
       </c>
       <c r="CC211" s="1" t="s">
+        <v>2186</v>
+      </c>
+      <c r="CD211" s="1" t="s">
         <v>2187</v>
       </c>
-      <c r="CD211" s="1" t="s">
+      <c r="CE211" s="1" t="s">
         <v>2188</v>
-      </c>
-      <c r="CE211" s="1" t="s">
-        <v>2189</v>
       </c>
     </row>
     <row r="212" spans="1:83" x14ac:dyDescent="0.25">
@@ -45708,13 +45690,13 @@
         <v>93</v>
       </c>
       <c r="K212" s="1" t="s">
+        <v>2189</v>
+      </c>
+      <c r="L212" s="1" t="s">
         <v>2190</v>
       </c>
-      <c r="L212" s="1" t="s">
+      <c r="N212" s="1" t="s">
         <v>2191</v>
-      </c>
-      <c r="N212" s="1" t="s">
-        <v>2192</v>
       </c>
       <c r="O212" s="1" t="s">
         <v>97</v>
@@ -45743,12 +45725,7 @@
       <c r="AA212" s="1">
         <v>0</v>
       </c>
-      <c r="AC212" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD212" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC212" s="3"/>
       <c r="AF212" s="1" t="s">
         <v>103</v>
       </c>
@@ -45798,7 +45775,7 @@
         <v>98</v>
       </c>
       <c r="AZ212" s="1" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="BB212" s="1">
         <v>1</v>
@@ -45816,10 +45793,10 @@
         <v>110</v>
       </c>
       <c r="BH212" s="1" t="s">
+        <v>2193</v>
+      </c>
+      <c r="BI212" s="1" t="s">
         <v>2194</v>
-      </c>
-      <c r="BI212" s="1" t="s">
-        <v>2195</v>
       </c>
       <c r="BM212" s="1" t="s">
         <v>113</v>
@@ -45828,7 +45805,7 @@
         <v>102</v>
       </c>
       <c r="BT212" s="1" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="BU212" s="1" t="s">
         <v>117</v>
@@ -45846,13 +45823,13 @@
         <v>98</v>
       </c>
       <c r="CC212" s="1" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="CD212" s="1" t="s">
         <v>1122</v>
       </c>
       <c r="CE212" s="1" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="213" spans="1:83" x14ac:dyDescent="0.25">
@@ -45887,13 +45864,13 @@
         <v>93</v>
       </c>
       <c r="K213" s="1" t="s">
+        <v>2198</v>
+      </c>
+      <c r="L213" s="1" t="s">
         <v>2199</v>
       </c>
-      <c r="L213" s="1" t="s">
+      <c r="N213" s="1" t="s">
         <v>2200</v>
-      </c>
-      <c r="N213" s="1" t="s">
-        <v>2201</v>
       </c>
       <c r="O213" s="1" t="s">
         <v>97</v>
@@ -45922,12 +45899,7 @@
       <c r="AA213" s="1">
         <v>0</v>
       </c>
-      <c r="AC213" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD213" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC213" s="3"/>
       <c r="AF213" s="1" t="s">
         <v>103</v>
       </c>
@@ -45977,7 +45949,7 @@
         <v>98</v>
       </c>
       <c r="AZ213" s="1" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="BB213" s="1">
         <v>1</v>
@@ -45995,7 +45967,7 @@
         <v>110</v>
       </c>
       <c r="BH213" s="1" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="BM213" s="1" t="s">
         <v>113</v>
@@ -46004,7 +45976,7 @@
         <v>102</v>
       </c>
       <c r="BT213" s="1" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="BU213" s="1" t="s">
         <v>117</v>
@@ -46025,10 +45997,10 @@
         <v>649</v>
       </c>
       <c r="CD213" s="1" t="s">
+        <v>2204</v>
+      </c>
+      <c r="CE213" s="1" t="s">
         <v>2205</v>
-      </c>
-      <c r="CE213" s="1" t="s">
-        <v>2206</v>
       </c>
     </row>
     <row r="214" spans="1:83" x14ac:dyDescent="0.25">
@@ -46063,13 +46035,13 @@
         <v>93</v>
       </c>
       <c r="K214" s="1" t="s">
+        <v>2206</v>
+      </c>
+      <c r="L214" s="1" t="s">
         <v>2207</v>
       </c>
-      <c r="L214" s="1" t="s">
+      <c r="N214" s="1" t="s">
         <v>2208</v>
-      </c>
-      <c r="N214" s="1" t="s">
-        <v>2209</v>
       </c>
       <c r="O214" s="1" t="s">
         <v>97</v>
@@ -46098,12 +46070,7 @@
       <c r="AA214" s="1">
         <v>0</v>
       </c>
-      <c r="AC214" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD214" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC214" s="3"/>
       <c r="AF214" s="1" t="s">
         <v>103</v>
       </c>
@@ -46153,7 +46120,7 @@
         <v>98</v>
       </c>
       <c r="AZ214" s="1" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="BB214" s="1">
         <v>1</v>
@@ -46171,10 +46138,10 @@
         <v>110</v>
       </c>
       <c r="BH214" s="1" t="s">
+        <v>2210</v>
+      </c>
+      <c r="BI214" s="1" t="s">
         <v>2211</v>
-      </c>
-      <c r="BI214" s="1" t="s">
-        <v>2212</v>
       </c>
       <c r="BM214" s="1" t="s">
         <v>113</v>
@@ -46183,7 +46150,7 @@
         <v>102</v>
       </c>
       <c r="BT214" s="1" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="BU214" s="1" t="s">
         <v>117</v>
@@ -46201,13 +46168,13 @@
         <v>98</v>
       </c>
       <c r="CC214" s="1" t="s">
+        <v>2213</v>
+      </c>
+      <c r="CD214" s="1" t="s">
+        <v>2213</v>
+      </c>
+      <c r="CE214" s="1" t="s">
         <v>2214</v>
-      </c>
-      <c r="CD214" s="1" t="s">
-        <v>2214</v>
-      </c>
-      <c r="CE214" s="1" t="s">
-        <v>2215</v>
       </c>
     </row>
     <row r="215" spans="1:83" x14ac:dyDescent="0.25">
@@ -46242,13 +46209,13 @@
         <v>93</v>
       </c>
       <c r="K215" s="1" t="s">
+        <v>2215</v>
+      </c>
+      <c r="L215" s="1" t="s">
         <v>2216</v>
       </c>
-      <c r="L215" s="1" t="s">
+      <c r="N215" s="1" t="s">
         <v>2217</v>
-      </c>
-      <c r="N215" s="1" t="s">
-        <v>2218</v>
       </c>
       <c r="O215" s="1" t="s">
         <v>97</v>
@@ -46283,12 +46250,7 @@
       <c r="AA215" s="1">
         <v>0</v>
       </c>
-      <c r="AC215" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD215" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC215" s="3"/>
       <c r="AF215" s="1" t="s">
         <v>103</v>
       </c>
@@ -46335,7 +46297,7 @@
         <v>98</v>
       </c>
       <c r="AZ215" s="1" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="BB215" s="1">
         <v>1</v>
@@ -46344,7 +46306,7 @@
         <v>18</v>
       </c>
       <c r="BD215" s="1" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="BE215" s="1" t="s">
         <v>108</v>
@@ -46356,7 +46318,7 @@
         <v>110</v>
       </c>
       <c r="BH215" s="1" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="BI215" s="1" t="s">
         <v>451</v>
@@ -46371,13 +46333,13 @@
         <v>114</v>
       </c>
       <c r="BR215" s="1" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="BS215" s="3">
         <v>35243</v>
       </c>
       <c r="BT215" s="1" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="BU215" s="1" t="s">
         <v>117</v>
@@ -46395,13 +46357,13 @@
         <v>98</v>
       </c>
       <c r="CC215" s="1" t="s">
+        <v>2223</v>
+      </c>
+      <c r="CD215" s="1" t="s">
         <v>2224</v>
       </c>
-      <c r="CD215" s="1" t="s">
+      <c r="CE215" s="1" t="s">
         <v>2225</v>
-      </c>
-      <c r="CE215" s="1" t="s">
-        <v>2226</v>
       </c>
     </row>
     <row r="216" spans="1:83" x14ac:dyDescent="0.25">
@@ -46436,13 +46398,13 @@
         <v>93</v>
       </c>
       <c r="K216" s="1" t="s">
+        <v>2226</v>
+      </c>
+      <c r="L216" s="1" t="s">
         <v>2227</v>
       </c>
-      <c r="L216" s="1" t="s">
+      <c r="N216" s="1" t="s">
         <v>2228</v>
-      </c>
-      <c r="N216" s="1" t="s">
-        <v>2229</v>
       </c>
       <c r="O216" s="1" t="s">
         <v>97</v>
@@ -46471,12 +46433,7 @@
       <c r="AA216" s="1">
         <v>0</v>
       </c>
-      <c r="AC216" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD216" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC216" s="3"/>
       <c r="AF216" s="1" t="s">
         <v>103</v>
       </c>
@@ -46526,7 +46483,7 @@
         <v>98</v>
       </c>
       <c r="AZ216" s="1" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="BB216" s="1">
         <v>1</v>
@@ -46544,10 +46501,10 @@
         <v>110</v>
       </c>
       <c r="BH216" s="1" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="BI216" s="1" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="BM216" s="1" t="s">
         <v>113</v>
@@ -46556,7 +46513,7 @@
         <v>102</v>
       </c>
       <c r="BT216" s="1" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
       <c r="BU216" s="1" t="s">
         <v>117</v>
@@ -46574,13 +46531,13 @@
         <v>98</v>
       </c>
       <c r="CC216" s="1" t="s">
+        <v>2232</v>
+      </c>
+      <c r="CD216" s="1" t="s">
         <v>2233</v>
       </c>
-      <c r="CD216" s="1" t="s">
+      <c r="CE216" s="1" t="s">
         <v>2234</v>
-      </c>
-      <c r="CE216" s="1" t="s">
-        <v>2235</v>
       </c>
     </row>
     <row r="217" spans="1:83" x14ac:dyDescent="0.25">
@@ -46615,13 +46572,13 @@
         <v>93</v>
       </c>
       <c r="K217" s="1" t="s">
+        <v>2235</v>
+      </c>
+      <c r="L217" s="1" t="s">
         <v>2236</v>
       </c>
-      <c r="L217" s="1" t="s">
+      <c r="N217" s="1" t="s">
         <v>2237</v>
-      </c>
-      <c r="N217" s="1" t="s">
-        <v>2238</v>
       </c>
       <c r="O217" s="1" t="s">
         <v>97</v>
@@ -46650,12 +46607,7 @@
       <c r="AA217" s="1">
         <v>0</v>
       </c>
-      <c r="AC217" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD217" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC217" s="3"/>
       <c r="AF217" s="1" t="s">
         <v>103</v>
       </c>
@@ -46705,7 +46657,7 @@
         <v>98</v>
       </c>
       <c r="AZ217" s="1" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="BB217" s="1">
         <v>1</v>
@@ -46723,7 +46675,7 @@
         <v>110</v>
       </c>
       <c r="BH217" s="1" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="BI217" s="1" t="s">
         <v>865</v>
@@ -46738,7 +46690,7 @@
         <v>152</v>
       </c>
       <c r="BT217" s="1" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="BU217" s="1" t="s">
         <v>117</v>
@@ -46756,13 +46708,13 @@
         <v>98</v>
       </c>
       <c r="CC217" s="1" t="s">
+        <v>2241</v>
+      </c>
+      <c r="CD217" s="1" t="s">
         <v>2242</v>
       </c>
-      <c r="CD217" s="1" t="s">
+      <c r="CE217" s="1" t="s">
         <v>2243</v>
-      </c>
-      <c r="CE217" s="1" t="s">
-        <v>2244</v>
       </c>
     </row>
     <row r="218" spans="1:83" x14ac:dyDescent="0.25">
@@ -46797,13 +46749,13 @@
         <v>93</v>
       </c>
       <c r="K218" s="1" t="s">
+        <v>2244</v>
+      </c>
+      <c r="L218" s="1" t="s">
         <v>2245</v>
       </c>
-      <c r="L218" s="1" t="s">
+      <c r="N218" s="1" t="s">
         <v>2246</v>
-      </c>
-      <c r="N218" s="1" t="s">
-        <v>2247</v>
       </c>
       <c r="O218" s="1" t="s">
         <v>97</v>
@@ -46832,12 +46784,7 @@
       <c r="AA218" s="1">
         <v>0</v>
       </c>
-      <c r="AC218" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD218" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC218" s="3"/>
       <c r="AF218" s="1" t="s">
         <v>103</v>
       </c>
@@ -46884,7 +46831,7 @@
         <v>98</v>
       </c>
       <c r="AZ218" s="1" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="BB218" s="1">
         <v>1</v>
@@ -46893,7 +46840,7 @@
         <v>18</v>
       </c>
       <c r="BD218" s="1" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
       <c r="BE218" s="1" t="s">
         <v>108</v>
@@ -46905,10 +46852,10 @@
         <v>110</v>
       </c>
       <c r="BH218" s="1" t="s">
+        <v>2249</v>
+      </c>
+      <c r="BI218" s="1" t="s">
         <v>2250</v>
-      </c>
-      <c r="BI218" s="1" t="s">
-        <v>2251</v>
       </c>
       <c r="BM218" s="1" t="s">
         <v>113</v>
@@ -46920,13 +46867,13 @@
         <v>211</v>
       </c>
       <c r="BR218" s="1" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="BS218" s="3">
         <v>34307</v>
       </c>
       <c r="BT218" s="1" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="BU218" s="1" t="s">
         <v>117</v>
@@ -46944,13 +46891,13 @@
         <v>98</v>
       </c>
       <c r="CC218" s="1" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
       <c r="CD218" s="1" t="s">
         <v>431</v>
       </c>
       <c r="CE218" s="1" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="219" spans="1:83" x14ac:dyDescent="0.25">
@@ -46985,13 +46932,13 @@
         <v>93</v>
       </c>
       <c r="K219" s="1" t="s">
+        <v>2255</v>
+      </c>
+      <c r="L219" s="1" t="s">
         <v>2256</v>
       </c>
-      <c r="L219" s="1" t="s">
+      <c r="N219" s="1" t="s">
         <v>2257</v>
-      </c>
-      <c r="N219" s="1" t="s">
-        <v>2258</v>
       </c>
       <c r="O219" s="1" t="s">
         <v>97</v>
@@ -47023,12 +46970,7 @@
       <c r="AA219" s="1">
         <v>0</v>
       </c>
-      <c r="AC219" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD219" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC219" s="3"/>
       <c r="AF219" s="1" t="s">
         <v>103</v>
       </c>
@@ -47078,7 +47020,7 @@
         <v>98</v>
       </c>
       <c r="AZ219" s="1" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="BB219" s="1">
         <v>1</v>
@@ -47099,10 +47041,10 @@
         <v>110</v>
       </c>
       <c r="BH219" s="1" t="s">
+        <v>2259</v>
+      </c>
+      <c r="BI219" s="1" t="s">
         <v>2260</v>
-      </c>
-      <c r="BI219" s="1" t="s">
-        <v>2261</v>
       </c>
       <c r="BM219" s="1" t="s">
         <v>113</v>
@@ -47111,7 +47053,7 @@
         <v>102</v>
       </c>
       <c r="BT219" s="1" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="BU219" s="1" t="s">
         <v>117</v>
@@ -47132,13 +47074,13 @@
         <v>98</v>
       </c>
       <c r="CC219" s="1" t="s">
+        <v>2262</v>
+      </c>
+      <c r="CD219" s="1" t="s">
         <v>2263</v>
       </c>
-      <c r="CD219" s="1" t="s">
+      <c r="CE219" s="1" t="s">
         <v>2264</v>
-      </c>
-      <c r="CE219" s="1" t="s">
-        <v>2265</v>
       </c>
     </row>
     <row r="220" spans="1:83" x14ac:dyDescent="0.25">
@@ -47173,13 +47115,13 @@
         <v>93</v>
       </c>
       <c r="K220" s="1" t="s">
+        <v>2265</v>
+      </c>
+      <c r="L220" s="1" t="s">
         <v>2266</v>
       </c>
-      <c r="L220" s="1" t="s">
+      <c r="N220" s="1" t="s">
         <v>2267</v>
-      </c>
-      <c r="N220" s="1" t="s">
-        <v>2268</v>
       </c>
       <c r="O220" s="1" t="s">
         <v>97</v>
@@ -47208,12 +47150,7 @@
       <c r="AA220" s="1">
         <v>0</v>
       </c>
-      <c r="AC220" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD220" s="1" t="s">
-        <v>2162</v>
-      </c>
+      <c r="AC220" s="3"/>
       <c r="AF220" s="1" t="s">
         <v>103</v>
       </c>
@@ -47260,7 +47197,7 @@
         <v>98</v>
       </c>
       <c r="AZ220" s="1" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="BB220" s="1">
         <v>1</v>
@@ -47281,10 +47218,10 @@
         <v>110</v>
       </c>
       <c r="BH220" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="BI220" s="1" t="s">
         <v>2270</v>
-      </c>
-      <c r="BI220" s="1" t="s">
-        <v>2271</v>
       </c>
       <c r="BM220" s="1" t="s">
         <v>113</v>
@@ -47296,13 +47233,13 @@
         <v>114</v>
       </c>
       <c r="BR220" s="1" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="BS220" s="3">
         <v>35950</v>
       </c>
       <c r="BT220" s="1" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
       <c r="BU220" s="1" t="s">
         <v>117</v>
@@ -47320,13 +47257,13 @@
         <v>98</v>
       </c>
       <c r="CC220" s="1" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="CD220" s="1" t="s">
         <v>1638</v>
       </c>
       <c r="CE220" s="1" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="221" spans="1:83" x14ac:dyDescent="0.25">
@@ -47361,13 +47298,13 @@
         <v>159</v>
       </c>
       <c r="K221" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="L221" s="1" t="s">
         <v>2276</v>
       </c>
-      <c r="L221" s="1" t="s">
+      <c r="N221" s="1" t="s">
         <v>2277</v>
-      </c>
-      <c r="N221" s="1" t="s">
-        <v>2278</v>
       </c>
       <c r="O221" s="1" t="s">
         <v>97</v>
@@ -47418,7 +47355,7 @@
         <v>0</v>
       </c>
       <c r="AN221" s="1" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="AO221" s="1">
         <v>0</v>
@@ -47463,13 +47400,13 @@
         <v>110</v>
       </c>
       <c r="BH221" s="1" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="BM221" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT221" s="1" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="BU221" s="1" t="s">
         <v>117</v>
@@ -47493,10 +47430,10 @@
         <v>2058</v>
       </c>
       <c r="CD221" s="1" t="s">
+        <v>2281</v>
+      </c>
+      <c r="CE221" s="1" t="s">
         <v>2282</v>
-      </c>
-      <c r="CE221" s="1" t="s">
-        <v>2283</v>
       </c>
     </row>
     <row r="222" spans="1:83" x14ac:dyDescent="0.25">
@@ -47531,13 +47468,13 @@
         <v>159</v>
       </c>
       <c r="K222" s="1" t="s">
+        <v>2283</v>
+      </c>
+      <c r="L222" s="1" t="s">
         <v>2284</v>
       </c>
-      <c r="L222" s="1" t="s">
+      <c r="N222" s="1" t="s">
         <v>2285</v>
-      </c>
-      <c r="N222" s="1" t="s">
-        <v>2286</v>
       </c>
       <c r="O222" s="1" t="s">
         <v>97</v>
@@ -47591,7 +47528,7 @@
         <v>0</v>
       </c>
       <c r="AN222" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="AO222" s="1">
         <v>0</v>
@@ -47636,13 +47573,13 @@
         <v>110</v>
       </c>
       <c r="BH222" s="1" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="BM222" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT222" s="1" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="BU222" s="1" t="s">
         <v>117</v>
@@ -47663,13 +47600,13 @@
         <v>98</v>
       </c>
       <c r="CC222" s="1" t="s">
+        <v>2288</v>
+      </c>
+      <c r="CD222" s="1" t="s">
         <v>2289</v>
       </c>
-      <c r="CD222" s="1" t="s">
+      <c r="CE222" s="1" t="s">
         <v>2290</v>
-      </c>
-      <c r="CE222" s="1" t="s">
-        <v>2291</v>
       </c>
     </row>
     <row r="223" spans="1:83" x14ac:dyDescent="0.25">
@@ -47704,13 +47641,13 @@
         <v>159</v>
       </c>
       <c r="K223" s="1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="L223" s="1" t="s">
         <v>2292</v>
       </c>
-      <c r="L223" s="1" t="s">
+      <c r="N223" s="1" t="s">
         <v>2293</v>
-      </c>
-      <c r="N223" s="1" t="s">
-        <v>2294</v>
       </c>
       <c r="O223" s="1" t="s">
         <v>97</v>
@@ -47764,7 +47701,7 @@
         <v>0</v>
       </c>
       <c r="AN223" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="AO223" s="1">
         <v>0</v>
@@ -47809,13 +47746,13 @@
         <v>110</v>
       </c>
       <c r="BH223" s="1" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="BM223" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT223" s="1" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="BU223" s="1" t="s">
         <v>117</v>
@@ -47836,13 +47773,13 @@
         <v>98</v>
       </c>
       <c r="CC223" s="1" t="s">
+        <v>2296</v>
+      </c>
+      <c r="CD223" s="1" t="s">
         <v>2297</v>
       </c>
-      <c r="CD223" s="1" t="s">
+      <c r="CE223" s="1" t="s">
         <v>2298</v>
-      </c>
-      <c r="CE223" s="1" t="s">
-        <v>2299</v>
       </c>
     </row>
     <row r="224" spans="1:83" x14ac:dyDescent="0.25">
@@ -47877,13 +47814,13 @@
         <v>159</v>
       </c>
       <c r="K224" s="1" t="s">
+        <v>2299</v>
+      </c>
+      <c r="L224" s="1" t="s">
         <v>2300</v>
       </c>
-      <c r="L224" s="1" t="s">
+      <c r="N224" s="1" t="s">
         <v>2301</v>
-      </c>
-      <c r="N224" s="1" t="s">
-        <v>2302</v>
       </c>
       <c r="O224" s="1" t="s">
         <v>97</v>
@@ -47979,13 +47916,13 @@
         <v>110</v>
       </c>
       <c r="BH224" s="1" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="BM224" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT224" s="1" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="BU224" s="1" t="s">
         <v>117</v>
@@ -48006,10 +47943,10 @@
         <v>98</v>
       </c>
       <c r="CC224" s="1" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="CD224" s="1" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="CE224" s="1" t="s">
         <v>199</v>
@@ -48047,13 +47984,13 @@
         <v>159</v>
       </c>
       <c r="K225" s="1" t="s">
+        <v>2305</v>
+      </c>
+      <c r="L225" s="1" t="s">
         <v>2306</v>
       </c>
-      <c r="L225" s="1" t="s">
+      <c r="N225" s="1" t="s">
         <v>2307</v>
-      </c>
-      <c r="N225" s="1" t="s">
-        <v>2308</v>
       </c>
       <c r="O225" s="1" t="s">
         <v>97</v>
@@ -48107,7 +48044,7 @@
         <v>0</v>
       </c>
       <c r="AN225" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="AO225" s="1">
         <v>0</v>
@@ -48152,13 +48089,13 @@
         <v>110</v>
       </c>
       <c r="BH225" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="BM225" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT225" s="1" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="BU225" s="1" t="s">
         <v>117</v>
@@ -48182,13 +48119,13 @@
         <v>98</v>
       </c>
       <c r="CC225" s="1" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="CD225" s="1" t="s">
         <v>1138</v>
       </c>
       <c r="CE225" s="1" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="226" spans="1:83" x14ac:dyDescent="0.25">
@@ -48223,13 +48160,13 @@
         <v>159</v>
       </c>
       <c r="K226" s="1" t="s">
+        <v>2312</v>
+      </c>
+      <c r="L226" s="1" t="s">
         <v>2313</v>
       </c>
-      <c r="L226" s="1" t="s">
+      <c r="N226" s="1" t="s">
         <v>2314</v>
-      </c>
-      <c r="N226" s="1" t="s">
-        <v>2315</v>
       </c>
       <c r="O226" s="1" t="s">
         <v>97</v>
@@ -48280,7 +48217,7 @@
         <v>0</v>
       </c>
       <c r="AN226" s="1" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="AO226" s="1">
         <v>0</v>
@@ -48325,13 +48262,13 @@
         <v>110</v>
       </c>
       <c r="BH226" s="1" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="BM226" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT226" s="1" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="BU226" s="1" t="s">
         <v>117</v>
@@ -48352,13 +48289,13 @@
         <v>98</v>
       </c>
       <c r="CC226" s="1" t="s">
+        <v>2318</v>
+      </c>
+      <c r="CD226" s="1" t="s">
+        <v>2233</v>
+      </c>
+      <c r="CE226" s="1" t="s">
         <v>2319</v>
-      </c>
-      <c r="CD226" s="1" t="s">
-        <v>2234</v>
-      </c>
-      <c r="CE226" s="1" t="s">
-        <v>2320</v>
       </c>
     </row>
     <row r="227" spans="1:83" x14ac:dyDescent="0.25">
@@ -48393,10 +48330,10 @@
         <v>93</v>
       </c>
       <c r="K227" s="1" t="s">
+        <v>2320</v>
+      </c>
+      <c r="L227" s="1" t="s">
         <v>2321</v>
-      </c>
-      <c r="L227" s="1" t="s">
-        <v>2322</v>
       </c>
       <c r="O227" s="1" t="s">
         <v>222</v>
@@ -48462,7 +48399,7 @@
         <v>16</v>
       </c>
       <c r="BD227" s="1" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="BX227" s="1">
         <v>0</v>
@@ -48480,7 +48417,7 @@
         <v>226</v>
       </c>
       <c r="CE227" s="1" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="228" spans="1:83" x14ac:dyDescent="0.25">
@@ -48509,16 +48446,16 @@
         <v>91</v>
       </c>
       <c r="I228" s="1" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="J228" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K228" s="1" t="s">
+        <v>2324</v>
+      </c>
+      <c r="L228" s="1" t="s">
         <v>2325</v>
-      </c>
-      <c r="L228" s="1" t="s">
-        <v>2326</v>
       </c>
       <c r="O228" s="1" t="s">
         <v>222</v>
@@ -48587,7 +48524,7 @@
         <v>0</v>
       </c>
       <c r="BZ228" s="1" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="CA228" s="1" t="s">
         <v>119</v>
@@ -48599,7 +48536,7 @@
         <v>226</v>
       </c>
       <c r="CE228" s="1" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="229" spans="1:83" x14ac:dyDescent="0.25">
@@ -48634,13 +48571,13 @@
         <v>93</v>
       </c>
       <c r="K229" s="1" t="s">
+        <v>2327</v>
+      </c>
+      <c r="L229" s="1" t="s">
         <v>2328</v>
       </c>
-      <c r="L229" s="1" t="s">
+      <c r="N229" s="1" t="s">
         <v>2329</v>
-      </c>
-      <c r="N229" s="1" t="s">
-        <v>2330</v>
       </c>
       <c r="O229" s="1" t="s">
         <v>97</v>
@@ -48718,7 +48655,7 @@
         <v>98</v>
       </c>
       <c r="AZ229" s="1" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="BB229" s="1">
         <v>1</v>
@@ -48736,7 +48673,7 @@
         <v>110</v>
       </c>
       <c r="BH229" s="1" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="BI229" s="1" t="s">
         <v>1032</v>
@@ -48751,7 +48688,7 @@
         <v>152</v>
       </c>
       <c r="BT229" s="1" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="BU229" s="1" t="s">
         <v>117</v>
@@ -48769,13 +48706,13 @@
         <v>98</v>
       </c>
       <c r="CC229" s="1" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="CD229" s="1" t="s">
         <v>431</v>
       </c>
       <c r="CE229" s="1" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="230" spans="1:83" x14ac:dyDescent="0.25">
@@ -48810,13 +48747,13 @@
         <v>93</v>
       </c>
       <c r="K230" s="1" t="s">
+        <v>2335</v>
+      </c>
+      <c r="L230" s="1" t="s">
         <v>2336</v>
       </c>
-      <c r="L230" s="1" t="s">
+      <c r="N230" s="1" t="s">
         <v>2337</v>
-      </c>
-      <c r="N230" s="1" t="s">
-        <v>2338</v>
       </c>
       <c r="O230" s="1" t="s">
         <v>97</v>
@@ -48891,7 +48828,7 @@
         <v>98</v>
       </c>
       <c r="AZ230" s="1" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="BB230" s="1">
         <v>1</v>
@@ -48909,10 +48846,10 @@
         <v>110</v>
       </c>
       <c r="BH230" s="1" t="s">
+        <v>2339</v>
+      </c>
+      <c r="BI230" s="1" t="s">
         <v>2340</v>
-      </c>
-      <c r="BI230" s="1" t="s">
-        <v>2341</v>
       </c>
       <c r="BM230" s="1" t="s">
         <v>113</v>
@@ -48924,13 +48861,13 @@
         <v>211</v>
       </c>
       <c r="BR230" s="1" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="BS230" s="3">
         <v>36099</v>
       </c>
       <c r="BT230" s="1" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="BU230" s="1" t="s">
         <v>117</v>
@@ -48948,13 +48885,13 @@
         <v>98</v>
       </c>
       <c r="CC230" s="1" t="s">
+        <v>2343</v>
+      </c>
+      <c r="CD230" s="1" t="s">
         <v>2344</v>
       </c>
-      <c r="CD230" s="1" t="s">
+      <c r="CE230" s="1" t="s">
         <v>2345</v>
-      </c>
-      <c r="CE230" s="1" t="s">
-        <v>2346</v>
       </c>
     </row>
     <row r="231" spans="1:83" x14ac:dyDescent="0.25">
@@ -48989,13 +48926,13 @@
         <v>93</v>
       </c>
       <c r="K231" s="1" t="s">
+        <v>2346</v>
+      </c>
+      <c r="L231" s="1" t="s">
         <v>2347</v>
       </c>
-      <c r="L231" s="1" t="s">
+      <c r="N231" s="1" t="s">
         <v>2348</v>
-      </c>
-      <c r="N231" s="1" t="s">
-        <v>2349</v>
       </c>
       <c r="O231" s="1" t="s">
         <v>97</v>
@@ -49070,7 +49007,7 @@
         <v>98</v>
       </c>
       <c r="AZ231" s="1" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="BB231" s="1">
         <v>1</v>
@@ -49088,7 +49025,7 @@
         <v>110</v>
       </c>
       <c r="BH231" s="1" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="BI231" s="1" t="s">
         <v>1695</v>
@@ -49103,13 +49040,13 @@
         <v>99</v>
       </c>
       <c r="BR231" s="1" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="BS231" s="3">
         <v>37735</v>
       </c>
       <c r="BT231" s="1" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="BU231" s="1" t="s">
         <v>117</v>
@@ -49127,13 +49064,13 @@
         <v>98</v>
       </c>
       <c r="CC231" s="1" t="s">
+        <v>2353</v>
+      </c>
+      <c r="CD231" s="1" t="s">
         <v>2354</v>
       </c>
-      <c r="CD231" s="1" t="s">
+      <c r="CE231" s="1" t="s">
         <v>2355</v>
-      </c>
-      <c r="CE231" s="1" t="s">
-        <v>2356</v>
       </c>
     </row>
     <row r="232" spans="1:83" x14ac:dyDescent="0.25">
@@ -49168,13 +49105,13 @@
         <v>93</v>
       </c>
       <c r="K232" s="1" t="s">
+        <v>2356</v>
+      </c>
+      <c r="L232" s="1" t="s">
         <v>2357</v>
       </c>
-      <c r="L232" s="1" t="s">
+      <c r="N232" s="1" t="s">
         <v>2358</v>
-      </c>
-      <c r="N232" s="1" t="s">
-        <v>2359</v>
       </c>
       <c r="O232" s="1" t="s">
         <v>97</v>
@@ -49252,7 +49189,7 @@
         <v>98</v>
       </c>
       <c r="AZ232" s="1" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="BB232" s="1">
         <v>1</v>
@@ -49270,7 +49207,7 @@
         <v>110</v>
       </c>
       <c r="BH232" s="1" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="BI232" s="1" t="s">
         <v>1032</v>
@@ -49282,7 +49219,7 @@
         <v>102</v>
       </c>
       <c r="BT232" s="1" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="BU232" s="1" t="s">
         <v>117</v>
@@ -49300,13 +49237,13 @@
         <v>98</v>
       </c>
       <c r="CC232" s="1" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="CD232" s="1" t="s">
         <v>817</v>
       </c>
       <c r="CE232" s="1" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="233" spans="1:83" x14ac:dyDescent="0.25">
@@ -49341,13 +49278,13 @@
         <v>93</v>
       </c>
       <c r="K233" s="1" t="s">
+        <v>2364</v>
+      </c>
+      <c r="L233" s="1" t="s">
         <v>2365</v>
       </c>
-      <c r="L233" s="1" t="s">
+      <c r="N233" s="1" t="s">
         <v>2366</v>
-      </c>
-      <c r="N233" s="1" t="s">
-        <v>2367</v>
       </c>
       <c r="O233" s="1" t="s">
         <v>97</v>
@@ -49380,7 +49317,7 @@
         <v>103</v>
       </c>
       <c r="AG233" s="1" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="AH233" s="1" t="s">
         <v>1735</v>
@@ -49425,7 +49362,7 @@
         <v>98</v>
       </c>
       <c r="AZ233" s="1" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="BB233" s="1">
         <v>1</v>
@@ -49443,7 +49380,7 @@
         <v>110</v>
       </c>
       <c r="BH233" s="1" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="BI233" s="1" t="s">
         <v>1671</v>
@@ -49455,7 +49392,7 @@
         <v>102</v>
       </c>
       <c r="BT233" s="1" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="BU233" s="1" t="s">
         <v>117</v>
@@ -49476,10 +49413,10 @@
         <v>1455</v>
       </c>
       <c r="CD233" s="1" t="s">
+        <v>2371</v>
+      </c>
+      <c r="CE233" s="1" t="s">
         <v>2372</v>
-      </c>
-      <c r="CE233" s="1" t="s">
-        <v>2373</v>
       </c>
     </row>
     <row r="234" spans="1:83" x14ac:dyDescent="0.25">
@@ -49514,13 +49451,13 @@
         <v>93</v>
       </c>
       <c r="K234" s="1" t="s">
+        <v>2373</v>
+      </c>
+      <c r="L234" s="1" t="s">
         <v>2374</v>
       </c>
-      <c r="L234" s="1" t="s">
+      <c r="N234" s="1" t="s">
         <v>2375</v>
-      </c>
-      <c r="N234" s="1" t="s">
-        <v>2376</v>
       </c>
       <c r="O234" s="1" t="s">
         <v>97</v>
@@ -49598,7 +49535,7 @@
         <v>98</v>
       </c>
       <c r="AZ234" s="1" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="BB234" s="1">
         <v>1</v>
@@ -49616,10 +49553,10 @@
         <v>110</v>
       </c>
       <c r="BH234" s="1" t="s">
+        <v>2377</v>
+      </c>
+      <c r="BI234" s="1" t="s">
         <v>2378</v>
-      </c>
-      <c r="BI234" s="1" t="s">
-        <v>2379</v>
       </c>
       <c r="BM234" s="1" t="s">
         <v>113</v>
@@ -49628,7 +49565,7 @@
         <v>102</v>
       </c>
       <c r="BT234" s="1" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="BU234" s="1" t="s">
         <v>117</v>
@@ -49652,7 +49589,7 @@
         <v>889</v>
       </c>
       <c r="CE234" s="1" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="235" spans="1:83" x14ac:dyDescent="0.25">
@@ -49687,13 +49624,13 @@
         <v>93</v>
       </c>
       <c r="K235" s="1" t="s">
+        <v>2381</v>
+      </c>
+      <c r="L235" s="1" t="s">
         <v>2382</v>
       </c>
-      <c r="L235" s="1" t="s">
+      <c r="N235" s="1" t="s">
         <v>2383</v>
-      </c>
-      <c r="N235" s="1" t="s">
-        <v>2384</v>
       </c>
       <c r="O235" s="1" t="s">
         <v>97</v>
@@ -49771,7 +49708,7 @@
         <v>98</v>
       </c>
       <c r="AZ235" s="1" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="BB235" s="1">
         <v>1</v>
@@ -49789,7 +49726,7 @@
         <v>110</v>
       </c>
       <c r="BH235" s="1" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="BI235" s="1" t="s">
         <v>580</v>
@@ -49801,7 +49738,7 @@
         <v>102</v>
       </c>
       <c r="BT235" s="1" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="BU235" s="1" t="s">
         <v>117</v>
@@ -49819,13 +49756,13 @@
         <v>98</v>
       </c>
       <c r="CC235" s="1" t="s">
+        <v>2387</v>
+      </c>
+      <c r="CD235" s="1" t="s">
         <v>2388</v>
       </c>
-      <c r="CD235" s="1" t="s">
+      <c r="CE235" s="1" t="s">
         <v>2389</v>
-      </c>
-      <c r="CE235" s="1" t="s">
-        <v>2390</v>
       </c>
     </row>
     <row r="236" spans="1:83" x14ac:dyDescent="0.25">
@@ -49860,13 +49797,13 @@
         <v>159</v>
       </c>
       <c r="K236" s="1" t="s">
+        <v>2390</v>
+      </c>
+      <c r="L236" s="1" t="s">
         <v>2391</v>
       </c>
-      <c r="L236" s="1" t="s">
+      <c r="N236" s="1" t="s">
         <v>2392</v>
-      </c>
-      <c r="N236" s="1" t="s">
-        <v>2393</v>
       </c>
       <c r="O236" s="1" t="s">
         <v>97</v>
@@ -49908,7 +49845,7 @@
         <v>0</v>
       </c>
       <c r="AN236" s="1" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="AO236" s="1">
         <v>0</v>
@@ -49947,13 +49884,13 @@
         <v>110</v>
       </c>
       <c r="BH236" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="BM236" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT236" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="BU236" s="1" t="s">
         <v>117</v>
@@ -49971,13 +49908,13 @@
         <v>98</v>
       </c>
       <c r="CC236" s="1" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="CD236" s="1" t="s">
         <v>302</v>
       </c>
       <c r="CE236" s="1" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="237" spans="1:83" x14ac:dyDescent="0.25">
@@ -50012,13 +49949,13 @@
         <v>93</v>
       </c>
       <c r="K237" s="1" t="s">
+        <v>2398</v>
+      </c>
+      <c r="L237" s="1" t="s">
         <v>2399</v>
       </c>
-      <c r="L237" s="1" t="s">
+      <c r="N237" s="1" t="s">
         <v>2400</v>
-      </c>
-      <c r="N237" s="1" t="s">
-        <v>2401</v>
       </c>
       <c r="O237" s="1" t="s">
         <v>97</v>
@@ -50057,7 +49994,7 @@
         <v>42247</v>
       </c>
       <c r="AD237" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="AF237" s="1" t="s">
         <v>103</v>
@@ -50111,7 +50048,7 @@
         <v>18</v>
       </c>
       <c r="BD237" s="1" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="BE237" s="1" t="s">
         <v>108</v>
@@ -50123,10 +50060,10 @@
         <v>110</v>
       </c>
       <c r="BH237" s="1" t="s">
+        <v>2402</v>
+      </c>
+      <c r="BI237" s="1" t="s">
         <v>2403</v>
-      </c>
-      <c r="BI237" s="1" t="s">
-        <v>2404</v>
       </c>
       <c r="BM237" s="1" t="s">
         <v>113</v>
@@ -50138,13 +50075,13 @@
         <v>211</v>
       </c>
       <c r="BR237" s="1" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="BS237" s="3">
         <v>36580</v>
       </c>
       <c r="BT237" s="1" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="BU237" s="1" t="s">
         <v>117</v>
@@ -50165,7 +50102,7 @@
         <v>98</v>
       </c>
       <c r="CC237" s="1" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="CD237" s="1" t="s">
         <v>292</v>
@@ -50206,13 +50143,13 @@
         <v>93</v>
       </c>
       <c r="K238" s="1" t="s">
+        <v>2407</v>
+      </c>
+      <c r="L238" s="1" t="s">
         <v>2408</v>
       </c>
-      <c r="L238" s="1" t="s">
+      <c r="N238" s="1" t="s">
         <v>2409</v>
-      </c>
-      <c r="N238" s="1" t="s">
-        <v>2410</v>
       </c>
       <c r="O238" s="1" t="s">
         <v>97</v>
@@ -50305,7 +50242,7 @@
         <v>110</v>
       </c>
       <c r="BH238" s="1" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="BI238" s="1" t="s">
         <v>388</v>
@@ -50320,13 +50257,13 @@
         <v>114</v>
       </c>
       <c r="BR238" s="1" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="BS238" s="3">
         <v>37747</v>
       </c>
       <c r="BT238" s="1" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="BU238" s="1" t="s">
         <v>117</v>
@@ -50350,7 +50287,7 @@
         <v>639</v>
       </c>
       <c r="CE238" s="1" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="239" spans="1:83" x14ac:dyDescent="0.25">
@@ -50385,13 +50322,13 @@
         <v>93</v>
       </c>
       <c r="K239" s="1" t="s">
+        <v>2414</v>
+      </c>
+      <c r="L239" s="1" t="s">
         <v>2415</v>
       </c>
-      <c r="L239" s="1" t="s">
+      <c r="N239" s="1" t="s">
         <v>2416</v>
-      </c>
-      <c r="N239" s="1" t="s">
-        <v>2417</v>
       </c>
       <c r="O239" s="1" t="s">
         <v>97</v>
@@ -50484,7 +50421,7 @@
         <v>110</v>
       </c>
       <c r="BH239" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="BM239" s="1" t="s">
         <v>113</v>
@@ -50493,7 +50430,7 @@
         <v>102</v>
       </c>
       <c r="BT239" s="1" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="BU239" s="1" t="s">
         <v>117</v>
@@ -50511,13 +50448,13 @@
         <v>98</v>
       </c>
       <c r="CC239" s="1" t="s">
+        <v>2419</v>
+      </c>
+      <c r="CD239" s="1" t="s">
         <v>2420</v>
       </c>
-      <c r="CD239" s="1" t="s">
+      <c r="CE239" s="1" t="s">
         <v>2421</v>
-      </c>
-      <c r="CE239" s="1" t="s">
-        <v>2422</v>
       </c>
     </row>
     <row r="240" spans="1:83" x14ac:dyDescent="0.25">
@@ -50552,13 +50489,13 @@
         <v>93</v>
       </c>
       <c r="K240" s="1" t="s">
+        <v>2422</v>
+      </c>
+      <c r="L240" s="1" t="s">
         <v>2423</v>
       </c>
-      <c r="L240" s="1" t="s">
+      <c r="N240" s="1" t="s">
         <v>2424</v>
-      </c>
-      <c r="N240" s="1" t="s">
-        <v>2425</v>
       </c>
       <c r="O240" s="1" t="s">
         <v>97</v>
@@ -50651,7 +50588,7 @@
         <v>110</v>
       </c>
       <c r="BH240" s="1" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="BI240" s="1" t="s">
         <v>580</v>
@@ -50663,7 +50600,7 @@
         <v>102</v>
       </c>
       <c r="BT240" s="1" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="BU240" s="1" t="s">
         <v>117</v>
@@ -50681,13 +50618,13 @@
         <v>98</v>
       </c>
       <c r="CC240" s="1" t="s">
+        <v>2427</v>
+      </c>
+      <c r="CD240" s="1" t="s">
         <v>2428</v>
       </c>
-      <c r="CD240" s="1" t="s">
+      <c r="CE240" s="1" t="s">
         <v>2429</v>
-      </c>
-      <c r="CE240" s="1" t="s">
-        <v>2430</v>
       </c>
     </row>
     <row r="241" spans="1:83" x14ac:dyDescent="0.25">
@@ -50722,13 +50659,13 @@
         <v>93</v>
       </c>
       <c r="K241" s="1" t="s">
+        <v>2430</v>
+      </c>
+      <c r="L241" s="1" t="s">
         <v>2431</v>
       </c>
-      <c r="L241" s="1" t="s">
+      <c r="N241" s="1" t="s">
         <v>2432</v>
-      </c>
-      <c r="N241" s="1" t="s">
-        <v>2433</v>
       </c>
       <c r="O241" s="1" t="s">
         <v>97</v>
@@ -50821,10 +50758,10 @@
         <v>110</v>
       </c>
       <c r="BH241" s="1" t="s">
+        <v>2433</v>
+      </c>
+      <c r="BI241" s="1" t="s">
         <v>2434</v>
-      </c>
-      <c r="BI241" s="1" t="s">
-        <v>2435</v>
       </c>
       <c r="BM241" s="1" t="s">
         <v>113</v>
@@ -50836,13 +50773,13 @@
         <v>99</v>
       </c>
       <c r="BR241" s="1" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="BS241" s="3">
         <v>37334</v>
       </c>
       <c r="BT241" s="1" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="BU241" s="1" t="s">
         <v>117</v>
@@ -50863,10 +50800,10 @@
         <v>514</v>
       </c>
       <c r="CD241" s="1" t="s">
+        <v>2437</v>
+      </c>
+      <c r="CE241" s="1" t="s">
         <v>2438</v>
-      </c>
-      <c r="CE241" s="1" t="s">
-        <v>2439</v>
       </c>
     </row>
     <row r="242" spans="1:83" x14ac:dyDescent="0.25">
@@ -50901,13 +50838,13 @@
         <v>93</v>
       </c>
       <c r="K242" s="1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="L242" s="1" t="s">
         <v>2440</v>
       </c>
-      <c r="L242" s="1" t="s">
+      <c r="N242" s="1" t="s">
         <v>2441</v>
-      </c>
-      <c r="N242" s="1" t="s">
-        <v>2442</v>
       </c>
       <c r="O242" s="1" t="s">
         <v>97</v>
@@ -51000,10 +50937,10 @@
         <v>110</v>
       </c>
       <c r="BH242" s="1" t="s">
+        <v>2442</v>
+      </c>
+      <c r="BI242" s="1" t="s">
         <v>2443</v>
-      </c>
-      <c r="BI242" s="1" t="s">
-        <v>2444</v>
       </c>
       <c r="BM242" s="1" t="s">
         <v>113</v>
@@ -51015,13 +50952,13 @@
         <v>99</v>
       </c>
       <c r="BR242" s="1" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="BS242" s="3">
         <v>37904</v>
       </c>
       <c r="BT242" s="1" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="BU242" s="1" t="s">
         <v>117</v>
@@ -51042,10 +50979,10 @@
         <v>889</v>
       </c>
       <c r="CD242" s="1" t="s">
+        <v>2446</v>
+      </c>
+      <c r="CE242" s="1" t="s">
         <v>2447</v>
-      </c>
-      <c r="CE242" s="1" t="s">
-        <v>2448</v>
       </c>
     </row>
     <row r="243" spans="1:83" x14ac:dyDescent="0.25">
@@ -51080,13 +51017,13 @@
         <v>93</v>
       </c>
       <c r="K243" s="1" t="s">
+        <v>2448</v>
+      </c>
+      <c r="L243" s="1" t="s">
         <v>2449</v>
       </c>
-      <c r="L243" s="1" t="s">
+      <c r="N243" s="1" t="s">
         <v>2450</v>
-      </c>
-      <c r="N243" s="1" t="s">
-        <v>2451</v>
       </c>
       <c r="O243" s="1" t="s">
         <v>97</v>
@@ -51176,7 +51113,7 @@
         <v>110</v>
       </c>
       <c r="BH243" s="1" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="BM243" s="1" t="s">
         <v>113</v>
@@ -51188,13 +51125,13 @@
         <v>114</v>
       </c>
       <c r="BR243" s="1" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="BS243" s="3">
         <v>36111</v>
       </c>
       <c r="BT243" s="1" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="BU243" s="1" t="s">
         <v>117</v>
@@ -51212,13 +51149,13 @@
         <v>98</v>
       </c>
       <c r="CC243" s="1" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="CD243" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="CE243" s="1" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="244" spans="1:83" x14ac:dyDescent="0.25">
@@ -51253,13 +51190,13 @@
         <v>93</v>
       </c>
       <c r="K244" s="1" t="s">
+        <v>2456</v>
+      </c>
+      <c r="L244" s="1" t="s">
         <v>2457</v>
       </c>
-      <c r="L244" s="1" t="s">
+      <c r="N244" s="1" t="s">
         <v>2458</v>
-      </c>
-      <c r="N244" s="1" t="s">
-        <v>2459</v>
       </c>
       <c r="O244" s="1" t="s">
         <v>97</v>
@@ -51352,10 +51289,10 @@
         <v>110</v>
       </c>
       <c r="BH244" s="1" t="s">
+        <v>2459</v>
+      </c>
+      <c r="BI244" s="1" t="s">
         <v>2460</v>
-      </c>
-      <c r="BI244" s="1" t="s">
-        <v>2461</v>
       </c>
       <c r="BM244" s="1" t="s">
         <v>113</v>
@@ -51367,13 +51304,13 @@
         <v>114</v>
       </c>
       <c r="BR244" s="1" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="BS244" s="3">
         <v>37785</v>
       </c>
       <c r="BT244" s="1" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="BU244" s="1" t="s">
         <v>117</v>
@@ -51391,13 +51328,13 @@
         <v>98</v>
       </c>
       <c r="CC244" s="1" t="s">
+        <v>2463</v>
+      </c>
+      <c r="CD244" s="1" t="s">
         <v>2464</v>
       </c>
-      <c r="CD244" s="1" t="s">
+      <c r="CE244" s="1" t="s">
         <v>2465</v>
-      </c>
-      <c r="CE244" s="1" t="s">
-        <v>2466</v>
       </c>
     </row>
     <row r="245" spans="1:83" x14ac:dyDescent="0.25">
@@ -51432,13 +51369,13 @@
         <v>93</v>
       </c>
       <c r="K245" s="1" t="s">
+        <v>2466</v>
+      </c>
+      <c r="L245" s="1" t="s">
         <v>2467</v>
       </c>
-      <c r="L245" s="1" t="s">
+      <c r="N245" s="1" t="s">
         <v>2468</v>
-      </c>
-      <c r="N245" s="1" t="s">
-        <v>2469</v>
       </c>
       <c r="O245" s="1" t="s">
         <v>97</v>
@@ -51531,7 +51468,7 @@
         <v>110</v>
       </c>
       <c r="BH245" s="1" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="BM245" s="1" t="s">
         <v>113</v>
@@ -51540,7 +51477,7 @@
         <v>102</v>
       </c>
       <c r="BT245" s="1" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="BU245" s="1" t="s">
         <v>117</v>
@@ -51561,10 +51498,10 @@
         <v>1154</v>
       </c>
       <c r="CD245" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="CE245" s="1" t="s">
         <v>2472</v>
-      </c>
-      <c r="CE245" s="1" t="s">
-        <v>2473</v>
       </c>
     </row>
     <row r="246" spans="1:83" x14ac:dyDescent="0.25">
@@ -51599,13 +51536,13 @@
         <v>93</v>
       </c>
       <c r="K246" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="L246" s="1" t="s">
         <v>2474</v>
       </c>
-      <c r="L246" s="1" t="s">
+      <c r="N246" s="1" t="s">
         <v>2475</v>
-      </c>
-      <c r="N246" s="1" t="s">
-        <v>2476</v>
       </c>
       <c r="O246" s="1" t="s">
         <v>97</v>
@@ -51683,7 +51620,7 @@
         <v>98</v>
       </c>
       <c r="AZ246" s="1" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="BB246" s="1">
         <v>1</v>
@@ -51713,7 +51650,7 @@
         <v>102</v>
       </c>
       <c r="BT246" s="1" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="BU246" s="1" t="s">
         <v>117</v>
@@ -51731,13 +51668,13 @@
         <v>98</v>
       </c>
       <c r="CC246" s="1" t="s">
+        <v>2478</v>
+      </c>
+      <c r="CD246" s="1" t="s">
         <v>2479</v>
       </c>
-      <c r="CD246" s="1" t="s">
+      <c r="CE246" s="1" t="s">
         <v>2480</v>
-      </c>
-      <c r="CE246" s="1" t="s">
-        <v>2481</v>
       </c>
     </row>
     <row r="247" spans="1:83" x14ac:dyDescent="0.25">
@@ -51772,13 +51709,13 @@
         <v>93</v>
       </c>
       <c r="K247" s="1" t="s">
+        <v>2481</v>
+      </c>
+      <c r="L247" s="1" t="s">
         <v>2482</v>
       </c>
-      <c r="L247" s="1" t="s">
+      <c r="N247" s="1" t="s">
         <v>2483</v>
-      </c>
-      <c r="N247" s="1" t="s">
-        <v>2484</v>
       </c>
       <c r="O247" s="1" t="s">
         <v>97</v>
@@ -51856,7 +51793,7 @@
         <v>98</v>
       </c>
       <c r="AZ247" s="1" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="BB247" s="1">
         <v>1</v>
@@ -51874,7 +51811,7 @@
         <v>110</v>
       </c>
       <c r="BH247" s="1" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="BI247" s="1" t="s">
         <v>1671</v>
@@ -51886,7 +51823,7 @@
         <v>102</v>
       </c>
       <c r="BT247" s="1" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="BU247" s="1" t="s">
         <v>117</v>
@@ -51904,13 +51841,13 @@
         <v>98</v>
       </c>
       <c r="CC247" s="1" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="CD247" s="1" t="s">
         <v>1025</v>
       </c>
       <c r="CE247" s="1" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="248" spans="1:83" x14ac:dyDescent="0.25">
@@ -51945,13 +51882,13 @@
         <v>93</v>
       </c>
       <c r="K248" s="1" t="s">
+        <v>2488</v>
+      </c>
+      <c r="L248" s="1" t="s">
         <v>2489</v>
       </c>
-      <c r="L248" s="1" t="s">
+      <c r="N248" s="1" t="s">
         <v>2490</v>
-      </c>
-      <c r="N248" s="1" t="s">
-        <v>2491</v>
       </c>
       <c r="O248" s="1" t="s">
         <v>97</v>
@@ -52029,7 +51966,7 @@
         <v>98</v>
       </c>
       <c r="AZ248" s="1" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="BB248" s="1">
         <v>1</v>
@@ -52047,7 +51984,7 @@
         <v>110</v>
       </c>
       <c r="BH248" s="1" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="BM248" s="1" t="s">
         <v>113</v>
@@ -52056,7 +51993,7 @@
         <v>102</v>
       </c>
       <c r="BT248" s="1" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="BU248" s="1" t="s">
         <v>117</v>
@@ -52077,10 +52014,10 @@
         <v>1025</v>
       </c>
       <c r="CD248" s="1" t="s">
+        <v>2494</v>
+      </c>
+      <c r="CE248" s="1" t="s">
         <v>2495</v>
-      </c>
-      <c r="CE248" s="1" t="s">
-        <v>2496</v>
       </c>
     </row>
     <row r="249" spans="1:83" x14ac:dyDescent="0.25">
@@ -52115,13 +52052,13 @@
         <v>93</v>
       </c>
       <c r="K249" s="1" t="s">
+        <v>2496</v>
+      </c>
+      <c r="L249" s="1" t="s">
         <v>2497</v>
       </c>
-      <c r="L249" s="1" t="s">
+      <c r="N249" s="1" t="s">
         <v>2498</v>
-      </c>
-      <c r="N249" s="1" t="s">
-        <v>2499</v>
       </c>
       <c r="O249" s="1" t="s">
         <v>97</v>
@@ -52196,7 +52133,7 @@
         <v>98</v>
       </c>
       <c r="AZ249" s="1" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="BB249" s="1">
         <v>1</v>
@@ -52217,7 +52154,7 @@
         <v>110</v>
       </c>
       <c r="BH249" s="1" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="BI249" s="1" t="s">
         <v>1671</v>
@@ -52232,13 +52169,13 @@
         <v>211</v>
       </c>
       <c r="BR249" s="1" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="BS249" s="3">
         <v>37513</v>
       </c>
       <c r="BT249" s="1" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="BU249" s="1" t="s">
         <v>117</v>
@@ -52256,13 +52193,13 @@
         <v>98</v>
       </c>
       <c r="CC249" s="1" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="CD249" s="1" t="s">
         <v>121</v>
       </c>
       <c r="CE249" s="1" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="250" spans="1:83" x14ac:dyDescent="0.25">
@@ -52297,13 +52234,13 @@
         <v>93</v>
       </c>
       <c r="K250" s="1" t="s">
+        <v>2505</v>
+      </c>
+      <c r="L250" s="1" t="s">
         <v>2506</v>
       </c>
-      <c r="L250" s="1" t="s">
+      <c r="N250" s="1" t="s">
         <v>2507</v>
-      </c>
-      <c r="N250" s="1" t="s">
-        <v>2508</v>
       </c>
       <c r="O250" s="1" t="s">
         <v>97</v>
@@ -52393,10 +52330,10 @@
         <v>110</v>
       </c>
       <c r="BH250" s="1" t="s">
+        <v>2508</v>
+      </c>
+      <c r="BI250" s="1" t="s">
         <v>2509</v>
-      </c>
-      <c r="BI250" s="1" t="s">
-        <v>2510</v>
       </c>
       <c r="BM250" s="1" t="s">
         <v>113</v>
@@ -52408,13 +52345,13 @@
         <v>99</v>
       </c>
       <c r="BR250" s="1" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="BS250" s="3">
         <v>41024</v>
       </c>
       <c r="BT250" s="1" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="BU250" s="1" t="s">
         <v>117</v>
@@ -52432,13 +52369,13 @@
         <v>98</v>
       </c>
       <c r="CC250" s="1" t="s">
+        <v>2512</v>
+      </c>
+      <c r="CD250" s="1" t="s">
         <v>2513</v>
       </c>
-      <c r="CD250" s="1" t="s">
+      <c r="CE250" s="1" t="s">
         <v>2514</v>
-      </c>
-      <c r="CE250" s="1" t="s">
-        <v>2515</v>
       </c>
     </row>
     <row r="251" spans="1:83" x14ac:dyDescent="0.25">
@@ -52473,13 +52410,13 @@
         <v>93</v>
       </c>
       <c r="K251" s="1" t="s">
+        <v>2515</v>
+      </c>
+      <c r="L251" s="1" t="s">
         <v>2516</v>
       </c>
-      <c r="L251" s="1" t="s">
+      <c r="N251" s="1" t="s">
         <v>2517</v>
-      </c>
-      <c r="N251" s="1" t="s">
-        <v>2518</v>
       </c>
       <c r="O251" s="1" t="s">
         <v>97</v>
@@ -52512,7 +52449,7 @@
         <v>103</v>
       </c>
       <c r="AG251" s="1" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="AH251" s="1" t="s">
         <v>1735</v>
@@ -52536,28 +52473,28 @@
         <v>97</v>
       </c>
       <c r="AQ251" s="1" t="s">
+        <v>2518</v>
+      </c>
+      <c r="AR251" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS251" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT251" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU251" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV251" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY251" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ251" s="1" t="s">
         <v>2519</v>
-      </c>
-      <c r="AR251" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS251" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT251" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU251" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV251" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY251" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ251" s="1" t="s">
-        <v>2520</v>
       </c>
       <c r="BB251" s="1">
         <v>1</v>
@@ -52575,7 +52512,7 @@
         <v>110</v>
       </c>
       <c r="BH251" s="1" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="BI251" s="1" t="s">
         <v>1032</v>
@@ -52590,13 +52527,13 @@
         <v>114</v>
       </c>
       <c r="BR251" s="1" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="BS251" s="3">
         <v>34808</v>
       </c>
       <c r="BT251" s="1" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="BU251" s="1" t="s">
         <v>117</v>
@@ -52614,13 +52551,13 @@
         <v>98</v>
       </c>
       <c r="CC251" s="1" t="s">
+        <v>2523</v>
+      </c>
+      <c r="CD251" s="1" t="s">
         <v>2524</v>
       </c>
-      <c r="CD251" s="1" t="s">
+      <c r="CE251" s="1" t="s">
         <v>2525</v>
-      </c>
-      <c r="CE251" s="1" t="s">
-        <v>2526</v>
       </c>
     </row>
     <row r="252" spans="1:83" x14ac:dyDescent="0.25">
@@ -52655,13 +52592,13 @@
         <v>93</v>
       </c>
       <c r="K252" s="1" t="s">
+        <v>2526</v>
+      </c>
+      <c r="L252" s="1" t="s">
         <v>2527</v>
       </c>
-      <c r="L252" s="1" t="s">
+      <c r="N252" s="1" t="s">
         <v>2528</v>
-      </c>
-      <c r="N252" s="1" t="s">
-        <v>2529</v>
       </c>
       <c r="O252" s="1" t="s">
         <v>97</v>
@@ -52736,7 +52673,7 @@
         <v>98</v>
       </c>
       <c r="AZ252" s="1" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="BB252" s="1">
         <v>1</v>
@@ -52754,7 +52691,7 @@
         <v>110</v>
       </c>
       <c r="BH252" s="1" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="BI252" s="1" t="s">
         <v>865</v>
@@ -52769,13 +52706,13 @@
         <v>99</v>
       </c>
       <c r="BR252" s="1" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="BS252" s="3">
         <v>37336</v>
       </c>
       <c r="BT252" s="1" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="BU252" s="1" t="s">
         <v>117</v>
@@ -52793,13 +52730,13 @@
         <v>98</v>
       </c>
       <c r="CC252" s="1" t="s">
+        <v>2533</v>
+      </c>
+      <c r="CD252" s="1" t="s">
         <v>2534</v>
       </c>
-      <c r="CD252" s="1" t="s">
+      <c r="CE252" s="1" t="s">
         <v>2535</v>
-      </c>
-      <c r="CE252" s="1" t="s">
-        <v>2536</v>
       </c>
     </row>
     <row r="253" spans="1:83" x14ac:dyDescent="0.25">
@@ -52834,13 +52771,13 @@
         <v>93</v>
       </c>
       <c r="K253" s="1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="L253" s="1" t="s">
         <v>2537</v>
       </c>
-      <c r="L253" s="1" t="s">
+      <c r="N253" s="1" t="s">
         <v>2538</v>
-      </c>
-      <c r="N253" s="1" t="s">
-        <v>2539</v>
       </c>
       <c r="O253" s="1" t="s">
         <v>97</v>
@@ -52918,7 +52855,7 @@
         <v>98</v>
       </c>
       <c r="AZ253" s="1" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="BB253" s="1">
         <v>1</v>
@@ -52936,10 +52873,10 @@
         <v>110</v>
       </c>
       <c r="BH253" s="1" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="BI253" s="1" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="BM253" s="1" t="s">
         <v>113</v>
@@ -52948,7 +52885,7 @@
         <v>102</v>
       </c>
       <c r="BT253" s="1" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="BU253" s="1" t="s">
         <v>117</v>
@@ -52966,13 +52903,13 @@
         <v>98</v>
       </c>
       <c r="CC253" s="1" t="s">
+        <v>2542</v>
+      </c>
+      <c r="CD253" s="1" t="s">
         <v>2543</v>
       </c>
-      <c r="CD253" s="1" t="s">
+      <c r="CE253" s="1" t="s">
         <v>2544</v>
-      </c>
-      <c r="CE253" s="1" t="s">
-        <v>2545</v>
       </c>
     </row>
     <row r="254" spans="1:83" x14ac:dyDescent="0.25">
@@ -53007,13 +52944,13 @@
         <v>93</v>
       </c>
       <c r="K254" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="L254" s="1" t="s">
         <v>2546</v>
       </c>
-      <c r="L254" s="1" t="s">
+      <c r="N254" s="1" t="s">
         <v>2547</v>
-      </c>
-      <c r="N254" s="1" t="s">
-        <v>2548</v>
       </c>
       <c r="O254" s="1" t="s">
         <v>97</v>
@@ -53106,7 +53043,7 @@
         <v>110</v>
       </c>
       <c r="BH254" s="1" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="BM254" s="1" t="s">
         <v>113</v>
@@ -53115,7 +53052,7 @@
         <v>102</v>
       </c>
       <c r="BT254" s="1" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="BU254" s="1" t="s">
         <v>117</v>
@@ -53133,13 +53070,13 @@
         <v>98</v>
       </c>
       <c r="CC254" s="1" t="s">
+        <v>2550</v>
+      </c>
+      <c r="CD254" s="1" t="s">
         <v>2551</v>
       </c>
-      <c r="CD254" s="1" t="s">
+      <c r="CE254" s="1" t="s">
         <v>2552</v>
-      </c>
-      <c r="CE254" s="1" t="s">
-        <v>2553</v>
       </c>
     </row>
     <row r="255" spans="1:83" x14ac:dyDescent="0.25">
@@ -53174,13 +53111,13 @@
         <v>159</v>
       </c>
       <c r="K255" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="L255" s="1" t="s">
         <v>2554</v>
       </c>
-      <c r="L255" s="1" t="s">
+      <c r="N255" s="1" t="s">
         <v>2555</v>
-      </c>
-      <c r="N255" s="1" t="s">
-        <v>2556</v>
       </c>
       <c r="O255" s="1" t="s">
         <v>97</v>
@@ -53267,7 +53204,7 @@
         <v>110</v>
       </c>
       <c r="BH255" s="1" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="BM255" s="1" t="s">
         <v>113</v>
@@ -53288,13 +53225,13 @@
         <v>98</v>
       </c>
       <c r="CC255" s="1" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="CD255" s="1" t="s">
         <v>2136</v>
       </c>
       <c r="CE255" s="1" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="256" spans="1:83" x14ac:dyDescent="0.25">
@@ -53323,7 +53260,7 @@
         <v>91</v>
       </c>
       <c r="I256" s="1" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="J256" s="1" t="s">
         <v>93</v>
@@ -53332,10 +53269,10 @@
         <v>254</v>
       </c>
       <c r="L256" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="M256" s="1" t="s">
         <v>2561</v>
-      </c>
-      <c r="M256" s="1" t="s">
-        <v>2562</v>
       </c>
       <c r="N256" s="1" t="s">
         <v>256</v>
@@ -53365,7 +53302,7 @@
         <v>42582</v>
       </c>
       <c r="AD256" s="1" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="AF256" s="1" t="s">
         <v>103</v>
@@ -53416,10 +53353,10 @@
         <v>257</v>
       </c>
       <c r="BH256" s="1" t="s">
+        <v>2563</v>
+      </c>
+      <c r="BI256" s="1" t="s">
         <v>2564</v>
-      </c>
-      <c r="BI256" s="1" t="s">
-        <v>2565</v>
       </c>
       <c r="BM256" s="1" t="s">
         <v>113</v>
@@ -53475,7 +53412,7 @@
         <v>123</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>89</v>
@@ -53493,16 +53430,16 @@
         <v>93</v>
       </c>
       <c r="K257" s="1" t="s">
+        <v>2566</v>
+      </c>
+      <c r="L257" s="1" t="s">
         <v>2567</v>
       </c>
-      <c r="L257" s="1" t="s">
+      <c r="M257" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="N257" s="1" t="s">
         <v>2568</v>
-      </c>
-      <c r="M257" s="1" t="s">
-        <v>2562</v>
-      </c>
-      <c r="N257" s="1" t="s">
-        <v>2569</v>
       </c>
       <c r="Q257" s="3">
         <v>17060</v>
@@ -53535,7 +53472,7 @@
         <v>42628</v>
       </c>
       <c r="AD257" s="1" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="AF257" s="1" t="s">
         <v>103</v>
@@ -53586,16 +53523,16 @@
         <v>98</v>
       </c>
       <c r="AZ257" s="1" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="BD257" s="1" t="s">
         <v>224</v>
       </c>
       <c r="BH257" s="1" t="s">
+        <v>2571</v>
+      </c>
+      <c r="BI257" s="1" t="s">
         <v>2572</v>
-      </c>
-      <c r="BI257" s="1" t="s">
-        <v>2573</v>
       </c>
       <c r="BM257" s="1" t="s">
         <v>113</v>
@@ -53604,7 +53541,7 @@
         <v>102</v>
       </c>
       <c r="BT257" s="1" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="BU257" s="1" t="s">
         <v>117</v>
@@ -53628,7 +53565,7 @@
         <v>121</v>
       </c>
       <c r="CE257" s="1" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="258" spans="1:83" x14ac:dyDescent="0.25">
@@ -53645,7 +53582,7 @@
         <v>123</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>98</v>
@@ -53657,22 +53594,22 @@
         <v>91</v>
       </c>
       <c r="I258" s="1" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="J258" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K258" s="1" t="s">
+        <v>2577</v>
+      </c>
+      <c r="L258" s="1" t="s">
         <v>2578</v>
       </c>
-      <c r="L258" s="1" t="s">
+      <c r="M258" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="N258" s="1" t="s">
         <v>2579</v>
-      </c>
-      <c r="M258" s="1" t="s">
-        <v>2562</v>
-      </c>
-      <c r="N258" s="1" t="s">
-        <v>2580</v>
       </c>
       <c r="Q258" s="3">
         <v>26864</v>
@@ -53702,7 +53639,7 @@
         <v>42735</v>
       </c>
       <c r="AD258" s="1" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="AF258" s="1" t="s">
         <v>103</v>
@@ -53753,7 +53690,7 @@
         <v>99</v>
       </c>
       <c r="BH258" s="1" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="BM258" s="1" t="s">
         <v>113</v>
@@ -53765,13 +53702,13 @@
         <v>211</v>
       </c>
       <c r="BR258" s="1" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="BS258" s="3">
         <v>102</v>
       </c>
       <c r="BT258" s="1" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="BU258" s="1" t="s">
         <v>117</v>
@@ -53792,13 +53729,13 @@
         <v>98</v>
       </c>
       <c r="CC258" s="1" t="s">
+        <v>2584</v>
+      </c>
+      <c r="CD258" s="1" t="s">
         <v>2585</v>
       </c>
-      <c r="CD258" s="1" t="s">
+      <c r="CE258" s="1" t="s">
         <v>2586</v>
-      </c>
-      <c r="CE258" s="1" t="s">
-        <v>2587</v>
       </c>
     </row>
     <row r="259" spans="1:83" x14ac:dyDescent="0.25">
@@ -53827,22 +53764,22 @@
         <v>91</v>
       </c>
       <c r="I259" s="1" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="J259" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K259" s="1" t="s">
+        <v>2587</v>
+      </c>
+      <c r="L259" s="1" t="s">
         <v>2588</v>
       </c>
-      <c r="L259" s="1" t="s">
+      <c r="M259" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="N259" s="1" t="s">
         <v>2589</v>
-      </c>
-      <c r="M259" s="1" t="s">
-        <v>2562</v>
-      </c>
-      <c r="N259" s="1" t="s">
-        <v>2590</v>
       </c>
       <c r="Q259" s="3">
         <v>17041</v>
@@ -53869,7 +53806,7 @@
         <v>42735</v>
       </c>
       <c r="AD259" s="1" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="AF259" s="1" t="s">
         <v>103</v>
@@ -53920,7 +53857,7 @@
         <v>98</v>
       </c>
       <c r="BH259" s="1" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="BM259" s="1" t="s">
         <v>113</v>
@@ -53929,7 +53866,7 @@
         <v>102</v>
       </c>
       <c r="BT259" s="1" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="BU259" s="1" t="s">
         <v>117</v>
@@ -53950,13 +53887,13 @@
         <v>98</v>
       </c>
       <c r="CC259" s="1" t="s">
+        <v>2592</v>
+      </c>
+      <c r="CD259" s="1" t="s">
         <v>2593</v>
       </c>
-      <c r="CD259" s="1" t="s">
+      <c r="CE259" s="1" t="s">
         <v>2594</v>
-      </c>
-      <c r="CE259" s="1" t="s">
-        <v>2595</v>
       </c>
     </row>
     <row r="260" spans="1:83" x14ac:dyDescent="0.25">
@@ -53991,16 +53928,16 @@
         <v>93</v>
       </c>
       <c r="K260" s="1" t="s">
+        <v>2595</v>
+      </c>
+      <c r="L260" s="1" t="s">
         <v>2596</v>
       </c>
-      <c r="L260" s="1" t="s">
+      <c r="M260" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="N260" s="1" t="s">
         <v>2597</v>
-      </c>
-      <c r="M260" s="1" t="s">
-        <v>2562</v>
-      </c>
-      <c r="N260" s="1" t="s">
-        <v>2598</v>
       </c>
       <c r="Q260" s="3">
         <v>25379</v>
@@ -54030,7 +53967,7 @@
         <v>39800</v>
       </c>
       <c r="AD260" s="1" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="AF260" s="1" t="s">
         <v>232</v>
@@ -54081,7 +54018,7 @@
         <v>99</v>
       </c>
       <c r="BH260" s="1" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="BM260" s="1" t="s">
         <v>113</v>
@@ -54093,13 +54030,13 @@
         <v>222</v>
       </c>
       <c r="BR260" s="1" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="BS260" s="3">
         <v>35915</v>
       </c>
       <c r="BT260" s="1" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="BU260" s="1" t="s">
         <v>117</v>
@@ -54114,7 +54051,7 @@
         <v>233</v>
       </c>
       <c r="BZ260" s="1" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="CA260" s="1" t="s">
         <v>119</v>
@@ -54129,7 +54066,7 @@
         <v>441</v>
       </c>
       <c r="CE260" s="1" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="261" spans="1:83" x14ac:dyDescent="0.25">
@@ -54164,16 +54101,16 @@
         <v>93</v>
       </c>
       <c r="K261" s="1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="L261" s="1" t="s">
         <v>2605</v>
       </c>
-      <c r="L261" s="1" t="s">
+      <c r="M261" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="N261" s="1" t="s">
         <v>2606</v>
-      </c>
-      <c r="M261" s="1" t="s">
-        <v>2562</v>
-      </c>
-      <c r="N261" s="1" t="s">
-        <v>2607</v>
       </c>
       <c r="Q261" s="3">
         <v>23750</v>
@@ -54202,12 +54139,7 @@
       <c r="AA261" s="1">
         <v>0</v>
       </c>
-      <c r="AC261" s="3">
-        <v>43008</v>
-      </c>
-      <c r="AD261" s="1" t="s">
-        <v>2608</v>
-      </c>
+      <c r="AC261" s="3"/>
       <c r="AF261" s="1" t="s">
         <v>103</v>
       </c>
@@ -54257,13 +54189,13 @@
         <v>98</v>
       </c>
       <c r="AZ261" s="1" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="BD261" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="BH261" s="1" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="BM261" s="1" t="s">
         <v>113</v>
@@ -54272,7 +54204,7 @@
         <v>102</v>
       </c>
       <c r="BT261" s="1" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="BU261" s="1" t="s">
         <v>117</v>
@@ -54296,10 +54228,10 @@
         <v>1065</v>
       </c>
       <c r="CD261" s="1" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
       <c r="CE261" s="1" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="262" spans="1:83" x14ac:dyDescent="0.25">
@@ -54334,13 +54266,13 @@
         <v>93</v>
       </c>
       <c r="K262" s="1" t="s">
+        <v>2612</v>
+      </c>
+      <c r="L262" s="1" t="s">
+        <v>2613</v>
+      </c>
+      <c r="N262" s="1" t="s">
         <v>2614</v>
-      </c>
-      <c r="L262" s="1" t="s">
-        <v>2615</v>
-      </c>
-      <c r="N262" s="1" t="s">
-        <v>2616</v>
       </c>
       <c r="O262" s="1" t="s">
         <v>97</v>
@@ -54430,13 +54362,13 @@
         <v>110</v>
       </c>
       <c r="BH262" s="1" t="s">
+        <v>2615</v>
+      </c>
+      <c r="BI262" s="1" t="s">
+        <v>2616</v>
+      </c>
+      <c r="BJ262" s="1" t="s">
         <v>2617</v>
-      </c>
-      <c r="BI262" s="1" t="s">
-        <v>2618</v>
-      </c>
-      <c r="BJ262" s="1" t="s">
-        <v>2619</v>
       </c>
       <c r="BM262" s="1" t="s">
         <v>113</v>
@@ -54445,13 +54377,13 @@
         <v>99</v>
       </c>
       <c r="BR262" s="1" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="BS262" s="3">
         <v>35209</v>
       </c>
       <c r="BT262" s="1" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="BU262" s="1" t="s">
         <v>117</v>
@@ -54472,10 +54404,10 @@
         <v>1515</v>
       </c>
       <c r="CD262" s="1" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="CE262" s="1" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="263" spans="1:83" x14ac:dyDescent="0.25">
@@ -54510,16 +54442,16 @@
         <v>93</v>
       </c>
       <c r="K263" s="1" t="s">
+        <v>2621</v>
+      </c>
+      <c r="L263" s="1" t="s">
+        <v>2622</v>
+      </c>
+      <c r="M263" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="N263" s="1" t="s">
         <v>2623</v>
-      </c>
-      <c r="L263" s="1" t="s">
-        <v>2624</v>
-      </c>
-      <c r="M263" s="1" t="s">
-        <v>2562</v>
-      </c>
-      <c r="N263" s="1" t="s">
-        <v>2625</v>
       </c>
       <c r="Q263" s="3">
         <v>17470</v>
@@ -54549,7 +54481,7 @@
         <v>43100</v>
       </c>
       <c r="AD263" s="1" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="AF263" s="1" t="s">
         <v>103</v>
@@ -54600,7 +54532,7 @@
         <v>98</v>
       </c>
       <c r="BH263" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
       <c r="BM263" s="1" t="s">
         <v>113</v>
@@ -54609,7 +54541,7 @@
         <v>102</v>
       </c>
       <c r="BT263" s="1" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="BU263" s="1" t="s">
         <v>117</v>
@@ -54624,7 +54556,7 @@
         <v>97</v>
       </c>
       <c r="BZ263" s="1" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="CA263" s="1" t="s">
         <v>119</v>
@@ -54633,13 +54565,13 @@
         <v>98</v>
       </c>
       <c r="CC263" s="1" t="s">
+        <v>2626</v>
+      </c>
+      <c r="CD263" s="1" t="s">
+        <v>2627</v>
+      </c>
+      <c r="CE263" s="1" t="s">
         <v>2628</v>
-      </c>
-      <c r="CD263" s="1" t="s">
-        <v>2629</v>
-      </c>
-      <c r="CE263" s="1" t="s">
-        <v>2630</v>
       </c>
     </row>
     <row r="264" spans="1:83" x14ac:dyDescent="0.25">
@@ -54674,7 +54606,7 @@
         <v>93</v>
       </c>
       <c r="K264" s="1" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="L264" s="1" t="s">
         <v>2140</v>
@@ -54683,7 +54615,7 @@
         <v>99</v>
       </c>
       <c r="N264" s="1" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="O264" s="1" t="s">
         <v>97</v>
@@ -54767,10 +54699,10 @@
         <v>110</v>
       </c>
       <c r="BH264" s="1" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="BI264" s="1" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
       <c r="BM264" s="1" t="s">
         <v>113</v>
@@ -54782,13 +54714,13 @@
         <v>99</v>
       </c>
       <c r="BR264" s="1" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="BS264" s="3">
         <v>34412</v>
       </c>
       <c r="BT264" s="1" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="BU264" s="1" t="s">
         <v>117</v>
@@ -54806,16 +54738,17 @@
         <v>98</v>
       </c>
       <c r="CC264" s="1" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="CD264" s="1" t="s">
         <v>2149</v>
       </c>
       <c r="CE264" s="1" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:CF264" xr:uid="{39558DF3-D8A8-43AF-BA09-01A4E695FDC1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>